<commit_message>
Added StROBe user behaviour
</commit_message>
<xml_diff>
--- a/misc/FlexibiltyFunctions/results/tables.xlsx
+++ b/misc/FlexibiltyFunctions/results/tables.xlsx
@@ -35,19 +35,19 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>NewStreet</t>
+    <t>New street</t>
   </si>
   <si>
-    <t>MixedStreet</t>
+    <t>Mixed street</t>
   </si>
   <si>
-    <t>OldStreet</t>
+    <t>Old street</t>
   </si>
   <si>
-    <t>linear</t>
+    <t>Series</t>
   </si>
   <si>
-    <t>radial</t>
+    <t>Parallel</t>
   </si>
   <si>
     <t>NoPipes</t>
@@ -477,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7530437207447092</v>
+        <v>1.506087441489418</v>
       </c>
       <c r="C5" t="n">
         <v>1020.082578953735</v>
       </c>
       <c r="D5" t="n">
-        <v>1020.83562267448</v>
+        <v>1021.588666395225</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -491,13 +491,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5955640062407849</v>
+        <v>1.19112801248157</v>
       </c>
       <c r="C6" t="n">
         <v>1020.082578953735</v>
       </c>
       <c r="D6" t="n">
-        <v>1020.678142959976</v>
+        <v>1021.273706966217</v>
       </c>
     </row>
   </sheetData>
@@ -541,19 +541,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>385.7964956788765</v>
+        <v>477.9511812611709</v>
       </c>
       <c r="C2" t="n">
-        <v>387.2329386709962</v>
+        <v>477.9494983402474</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01110402476751915</v>
+        <v>6.098616604813287</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09746728546178929</v>
+        <v>2.7114429284793</v>
       </c>
       <c r="F2" t="n">
-        <v>387.330405956458</v>
+        <v>480.6609412687267</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -561,19 +561,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>380.7882839622944</v>
+        <v>339.4231819081451</v>
       </c>
       <c r="C3" t="n">
-        <v>380.5221840208742</v>
+        <v>339.4231819057059</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2300238905081642</v>
+        <v>5.876741577525536</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6477143322636039</v>
+        <v>2.421182327281713</v>
       </c>
       <c r="F3" t="n">
-        <v>381.1698983531378</v>
+        <v>341.8443642329876</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -581,19 +581,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>372.0174581982956</v>
+        <v>207.8950470401323</v>
       </c>
       <c r="C4" t="n">
-        <v>372.7242787690247</v>
+        <v>207.8937435944281</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3873981816668675</v>
+        <v>5.738490564899621</v>
       </c>
       <c r="E4" t="n">
-        <v>1.091930966353175</v>
+        <v>2.360365328902844</v>
       </c>
       <c r="F4" t="n">
-        <v>373.8162097353779</v>
+        <v>210.2541089233309</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -601,19 +601,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>1669.758733198825</v>
+        <v>1212.022556714328</v>
       </c>
       <c r="C5" t="n">
-        <v>1760.191479449491</v>
+        <v>1212.022556714306</v>
       </c>
       <c r="D5" t="n">
-        <v>2.32724134140517</v>
+        <v>27.69522036387207</v>
       </c>
       <c r="E5" t="n">
-        <v>2.419278736753768</v>
+        <v>21.56055993229165</v>
       </c>
       <c r="F5" t="n">
-        <v>1762.610758186245</v>
+        <v>1233.583116646598</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -621,19 +621,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>1669.758733198825</v>
+        <v>1212.022556714328</v>
       </c>
       <c r="C6" t="n">
-        <v>1741.192818311793</v>
+        <v>1212.02255671423</v>
       </c>
       <c r="D6" t="n">
-        <v>1.039757154663675</v>
+        <v>13.21454909548265</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8784699928692135</v>
+        <v>9.77959530350563</v>
       </c>
       <c r="F6" t="n">
-        <v>1742.071288304662</v>
+        <v>1221.802152017735</v>
       </c>
     </row>
   </sheetData>
@@ -677,19 +677,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>579.5140426636555</v>
+        <v>728.1378986128668</v>
       </c>
       <c r="C2" t="n">
-        <v>594.6934396468271</v>
+        <v>728.0536107133894</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3514007368333344</v>
+        <v>6.625455132925002</v>
       </c>
       <c r="E2" t="n">
-        <v>2.267358456956484</v>
+        <v>4.888157839120087</v>
       </c>
       <c r="F2" t="n">
-        <v>596.9607981037835</v>
+        <v>732.9417685525095</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -697,19 +697,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>597.4305958031335</v>
+        <v>567.3792269942551</v>
       </c>
       <c r="C3" t="n">
-        <v>602.604524868644</v>
+        <v>567.3792269928329</v>
       </c>
       <c r="D3" t="n">
-        <v>1.541971013309421</v>
+        <v>6.490536311924996</v>
       </c>
       <c r="E3" t="n">
-        <v>3.053954837389351</v>
+        <v>4.795462583408751</v>
       </c>
       <c r="F3" t="n">
-        <v>605.6584797060334</v>
+        <v>572.1746895762416</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -717,19 +717,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>606.4448700444664</v>
+        <v>413.7448922070051</v>
       </c>
       <c r="C4" t="n">
-        <v>607.2282963562053</v>
+        <v>413.58855031634</v>
       </c>
       <c r="D4" t="n">
-        <v>1.878959421050163</v>
+        <v>6.456398948808332</v>
       </c>
       <c r="E4" t="n">
-        <v>3.507054537282813</v>
+        <v>4.74442293016145</v>
       </c>
       <c r="F4" t="n">
-        <v>610.7353508934881</v>
+        <v>418.3329732465015</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -737,19 +737,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>2397.630113425227</v>
+        <v>2035.489665051741</v>
       </c>
       <c r="C5" t="n">
-        <v>2500.820925594765</v>
+        <v>2035.489665051741</v>
       </c>
       <c r="D5" t="n">
-        <v>3.895419806220104</v>
+        <v>28.96880013744834</v>
       </c>
       <c r="E5" t="n">
-        <v>4.443764496491101</v>
+        <v>25.87363108599965</v>
       </c>
       <c r="F5" t="n">
-        <v>2505.264690091255</v>
+        <v>2061.363296137741</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -757,19 +757,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>2397.630113425227</v>
+        <v>2035.489665051741</v>
       </c>
       <c r="C6" t="n">
-        <v>2480.907085448521</v>
+        <v>2035.489665051741</v>
       </c>
       <c r="D6" t="n">
-        <v>2.001758678579358</v>
+        <v>13.78667678452683</v>
       </c>
       <c r="E6" t="n">
-        <v>2.405980433065935</v>
+        <v>12.08802500770862</v>
       </c>
       <c r="F6" t="n">
-        <v>2483.313065881587</v>
+        <v>2047.57769005945</v>
       </c>
     </row>
   </sheetData>
@@ -813,19 +813,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>773.2315896484323</v>
+        <v>978.3246159645652</v>
       </c>
       <c r="C2" t="n">
-        <v>802.1539406226625</v>
+        <v>978.1577230865371</v>
       </c>
       <c r="D2" t="n">
-        <v>0.691697448908333</v>
+        <v>7.152293661016666</v>
       </c>
       <c r="E2" t="n">
-        <v>4.437249628458333</v>
+        <v>7.06487274975</v>
       </c>
       <c r="F2" t="n">
-        <v>806.5911902511208</v>
+        <v>985.222595836287</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -833,19 +833,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>814.0729076439725</v>
+        <v>795.3352720803679</v>
       </c>
       <c r="C3" t="n">
-        <v>824.6868657164251</v>
+        <v>795.335272079975</v>
       </c>
       <c r="D3" t="n">
-        <v>2.853918136107166</v>
+        <v>7.104331046333335</v>
       </c>
       <c r="E3" t="n">
-        <v>5.460195342508333</v>
+        <v>7.169742839516664</v>
       </c>
       <c r="F3" t="n">
-        <v>830.1470610589334</v>
+        <v>802.5050149194916</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -853,19 +853,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>840.8722818906374</v>
+        <v>619.5947373738678</v>
       </c>
       <c r="C4" t="n">
-        <v>841.7323139433398</v>
+        <v>619.2833570382555</v>
       </c>
       <c r="D4" t="n">
-        <v>3.370520660430584</v>
+        <v>7.174307332708334</v>
       </c>
       <c r="E4" t="n">
-        <v>5.922178108224999</v>
+        <v>7.128480531408336</v>
       </c>
       <c r="F4" t="n">
-        <v>847.6544920515648</v>
+        <v>626.4118375696638</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -873,19 +873,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>3125.501493651601</v>
+        <v>2858.956773389188</v>
       </c>
       <c r="C5" t="n">
-        <v>3241.450371740041</v>
+        <v>2858.956773389189</v>
       </c>
       <c r="D5" t="n">
-        <v>5.463598271062825</v>
+        <v>30.24237991109465</v>
       </c>
       <c r="E5" t="n">
-        <v>6.468250256322169</v>
+        <v>30.18670223978383</v>
       </c>
       <c r="F5" t="n">
-        <v>3247.918621996364</v>
+        <v>2889.143475628972</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -893,19 +893,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>3125.501493651601</v>
+        <v>2858.956773389188</v>
       </c>
       <c r="C6" t="n">
-        <v>3220.621352585273</v>
+        <v>2858.956773389188</v>
       </c>
       <c r="D6" t="n">
-        <v>2.963760202334127</v>
+        <v>14.35880447359172</v>
       </c>
       <c r="E6" t="n">
-        <v>3.933490873144513</v>
+        <v>14.39645471192019</v>
       </c>
       <c r="F6" t="n">
-        <v>3224.554843458417</v>
+        <v>2873.353228101108</v>
       </c>
     </row>
   </sheetData>
@@ -949,19 +949,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>70</v>
+        <v>114.148285396</v>
       </c>
       <c r="C2" t="n">
-        <v>53.88716666669</v>
+        <v>114.25449989113</v>
       </c>
       <c r="D2" t="n">
-        <v>2.943590311099999</v>
+        <v>22.75799457469999</v>
       </c>
       <c r="E2" t="n">
-        <v>12.2449672142</v>
+        <v>21.8219291373</v>
       </c>
       <c r="F2" t="n">
-        <v>53.88716666669</v>
+        <v>114.25449989113</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -969,19 +969,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>48.2907908253</v>
+        <v>109.60337307274</v>
       </c>
       <c r="C3" t="n">
-        <v>60.88716666663</v>
+        <v>109.60337307287</v>
       </c>
       <c r="D3" t="n">
-        <v>3.8747372617</v>
+        <v>19.21533658469999</v>
       </c>
       <c r="E3" t="n">
-        <v>15.3400650467</v>
+        <v>20.6092917201</v>
       </c>
       <c r="F3" t="n">
-        <v>61.48092148843</v>
+        <v>109.60337307287</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -989,19 +989,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>60.16015098690001</v>
+        <v>107.81158514048</v>
       </c>
       <c r="C4" t="n">
-        <v>65.8785199453</v>
+        <v>107.80596518561</v>
       </c>
       <c r="D4" t="n">
-        <v>3.7164204379</v>
+        <v>17.6087516207</v>
       </c>
       <c r="E4" t="n">
-        <v>18.38280532280001</v>
+        <v>19.420590118</v>
       </c>
       <c r="F4" t="n">
-        <v>73.75210118788</v>
+        <v>107.80596518561</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1009,19 +1009,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>190.1922358870569</v>
+        <v>335.341277757649</v>
       </c>
       <c r="C5" t="n">
-        <v>219.5545</v>
+        <v>335.341277757649</v>
       </c>
       <c r="D5" t="n">
-        <v>8.612486212553341</v>
+        <v>65.79397546363202</v>
       </c>
       <c r="E5" t="n">
-        <v>39.25682347170054</v>
+        <v>64.04184993928159</v>
       </c>
       <c r="F5" t="n">
-        <v>219.5545</v>
+        <v>335.341277757649</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1029,19 +1029,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>190.1922358870569</v>
+        <v>335.341277757649</v>
       </c>
       <c r="C6" t="n">
-        <v>225.6276508430201</v>
+        <v>335.341277757649</v>
       </c>
       <c r="D6" t="n">
-        <v>8.689659568871313</v>
+        <v>54.29547261951701</v>
       </c>
       <c r="E6" t="n">
-        <v>32.94317456523864</v>
+        <v>63.19183769733179</v>
       </c>
       <c r="F6" t="n">
-        <v>225.6276508430201</v>
+        <v>335.341277757649</v>
       </c>
     </row>
   </sheetData>
@@ -1085,19 +1085,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>2.645901987933038</v>
+        <v>3.347704725050633</v>
       </c>
       <c r="C2" t="n">
-        <v>2.744870662988343</v>
+        <v>3.347133638452959</v>
       </c>
       <c r="D2" t="n">
-        <v>1.658330091342648</v>
+        <v>17.14747368072926</v>
       </c>
       <c r="E2" t="n">
-        <v>10.63821269441549</v>
+        <v>16.93788388392589</v>
       </c>
       <c r="F2" t="n">
-        <v>2.756120619938396</v>
+        <v>3.366503805686526</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1105,19 +1105,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>2.084300828605334</v>
+        <v>2.036326170605284</v>
       </c>
       <c r="C3" t="n">
-        <v>2.111476136120752</v>
+        <v>2.036326170604278</v>
       </c>
       <c r="D3" t="n">
-        <v>6.842208729849229</v>
+        <v>17.03248432040363</v>
       </c>
       <c r="E3" t="n">
-        <v>13.09070353719135</v>
+        <v>17.18930771932724</v>
       </c>
       <c r="F3" t="n">
-        <v>2.123188660942577</v>
+        <v>2.052491212645102</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1125,19 +1125,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>1.719892462739846</v>
+        <v>1.267298663200775</v>
       </c>
       <c r="C4" t="n">
-        <v>1.721651543966584</v>
+        <v>1.266661776120776</v>
       </c>
       <c r="D4" t="n">
-        <v>6.843803388253278</v>
+        <v>14.56734842434912</v>
       </c>
       <c r="E4" t="n">
-        <v>12.02491445275161</v>
+        <v>14.47429763202149</v>
       </c>
       <c r="F4" t="n">
-        <v>1.732019860584674</v>
+        <v>1.279952803588751</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1145,19 +1145,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>3.063969092440853</v>
+        <v>2.802671893800524</v>
       </c>
       <c r="C5" t="n">
-        <v>3.177635260730253</v>
+        <v>2.802671893800525</v>
       </c>
       <c r="D5" t="n">
-        <v>7.255353335473931</v>
+        <v>20.0800956690715</v>
       </c>
       <c r="E5" t="n">
-        <v>8.589475057205853</v>
+        <v>20.04312725025529</v>
       </c>
       <c r="F5" t="n">
-        <v>3.181627433305241</v>
+        <v>2.828088809778594</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1165,19 +1165,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>3.063969092440853</v>
+        <v>2.802671893800524</v>
       </c>
       <c r="C6" t="n">
-        <v>3.157216306829352</v>
+        <v>2.802671893800524</v>
       </c>
       <c r="D6" t="n">
-        <v>4.976392413372085</v>
+        <v>12.05479538985646</v>
       </c>
       <c r="E6" t="n">
-        <v>6.604648420533012</v>
+        <v>12.08640428321968</v>
       </c>
       <c r="F6" t="n">
-        <v>3.159227877758975</v>
+        <v>2.813499660768371</v>
       </c>
     </row>
   </sheetData>
@@ -1221,19 +1221,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.177083333333333</v>
+        <v>0.8125</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.01736111111111111</v>
+        <v>0.02430555555555556</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1.177083333333333</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1241,19 +1241,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.9895833333333334</v>
+        <v>0.8020833333333334</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>1.0625</v>
+        <v>0.8020833333333334</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.03125</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>1.0625</v>
+        <v>0.8020833333333334</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1261,19 +1261,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6979166666666667</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.8541666666666666</v>
+        <v>0.6979166666666667</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.03472222222222222</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.8541666666666666</v>
+        <v>0.6979166666666667</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1281,19 +1281,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1.083333333333333</v>
+        <v>1.270833333333333</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1.291666666666667</v>
+        <v>1.270833333333333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.2048611111111111</v>
+        <v>0.0451388888888889</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.01736111111111111</v>
+        <v>0.03819444444444445</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>1.291666666666667</v>
+        <v>1.270833333333333</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1301,19 +1301,19 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>1.083333333333333</v>
+        <v>1.270833333333333</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1.291666666666667</v>
+        <v>1.270833333333333</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.2048611111111111</v>
+        <v>0.02430555555555556</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.01041666666666667</v>
+        <v>0.02083333333333333</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1.291666666666667</v>
+        <v>1.270833333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1357,19 +1357,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>193.7175469847807</v>
+        <v>250.1867173516957</v>
       </c>
       <c r="C2" t="n">
-        <v>207.4605009758361</v>
+        <v>250.104112373142</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3402967120746325</v>
+        <v>0.5268385280915027</v>
       </c>
       <c r="E2" t="n">
-        <v>2.169891171502968</v>
+        <v>2.176714910625378</v>
       </c>
       <c r="F2" t="n">
-        <v>209.6303921473391</v>
+        <v>252.2808272837674</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1377,19 +1377,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>216.6423118408402</v>
+        <v>227.9560450861154</v>
       </c>
       <c r="C3" t="n">
-        <v>222.0823408477745</v>
+        <v>227.9560450871386</v>
       </c>
       <c r="D3" t="n">
-        <v>1.311947122794663</v>
+        <v>0.6137947344095664</v>
       </c>
       <c r="E3" t="n">
-        <v>2.406240505117239</v>
+        <v>2.374280256109159</v>
       </c>
       <c r="F3" t="n">
-        <v>224.4885813528917</v>
+        <v>230.3303253432478</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1397,19 +1397,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>234.4274118461808</v>
+        <v>205.8498451668565</v>
       </c>
       <c r="C4" t="n">
-        <v>234.5040175871354</v>
+        <v>205.6948067219164</v>
       </c>
       <c r="D4" t="n">
-        <v>1.491561239381554</v>
+        <v>0.7179083839009763</v>
       </c>
       <c r="E4" t="n">
-        <v>2.415123570942342</v>
+        <v>2.38405760124715</v>
       </c>
       <c r="F4" t="n">
-        <v>236.9191411580778</v>
+        <v>208.0788643231635</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1417,19 +1417,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>727.8713802263755</v>
+        <v>823.4671083374342</v>
       </c>
       <c r="C5" t="n">
-        <v>740.6294461452617</v>
+        <v>823.4671083374633</v>
       </c>
       <c r="D5" t="n">
-        <v>1.568178464840457</v>
+        <v>1.273579773649544</v>
       </c>
       <c r="E5" t="n">
-        <v>2.024485759837262</v>
+        <v>4.313071153785131</v>
       </c>
       <c r="F5" t="n">
-        <v>742.6539319050989</v>
+        <v>827.7801794912484</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1437,19 +1437,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>727.8713802263755</v>
+        <v>823.4671083374342</v>
       </c>
       <c r="C6" t="n">
-        <v>739.7142671367492</v>
+        <v>823.4671083374888</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9620015237578627</v>
+        <v>0.5721276890690206</v>
       </c>
       <c r="E6" t="n">
-        <v>1.527510440086189</v>
+        <v>2.308429704196897</v>
       </c>
       <c r="F6" t="n">
-        <v>741.2417775768354</v>
+        <v>825.7755380416856</v>
       </c>
     </row>
   </sheetData>
@@ -1493,19 +1493,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>74.94702110222832</v>
+        <v>74.42702419321479</v>
       </c>
       <c r="C2" t="n">
-        <v>74.1370713936108</v>
+        <v>74.43110589724748</v>
       </c>
       <c r="D2" t="n">
-        <v>50.80266478933871</v>
+        <v>92.63399191941015</v>
       </c>
       <c r="E2" t="n">
-        <v>51.09828489034696</v>
+        <v>69.18960909240955</v>
       </c>
       <c r="F2" t="n">
-        <v>74.01032955953661</v>
+        <v>74.39351996688852</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1513,19 +1513,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>73.38784894972584</v>
+        <v>71.33837098780256</v>
       </c>
       <c r="C3" t="n">
-        <v>73.07070718828733</v>
+        <v>71.33837098765898</v>
       </c>
       <c r="D3" t="n">
-        <v>54.02996649625059</v>
+        <v>91.36027401709086</v>
       </c>
       <c r="E3" t="n">
-        <v>55.93123771698426</v>
+        <v>66.88472222893816</v>
       </c>
       <c r="F3" t="n">
-        <v>72.95797432959979</v>
+        <v>71.29858118493253</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1533,19 +1533,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>72.12092527062492</v>
+        <v>66.77669567691645</v>
       </c>
       <c r="C4" t="n">
-        <v>72.14030948993111</v>
+        <v>66.78502588761208</v>
       </c>
       <c r="D4" t="n">
-        <v>55.74685960395976</v>
+        <v>89.99334219309334</v>
       </c>
       <c r="E4" t="n">
-        <v>59.21899802067521</v>
+        <v>66.55587973610642</v>
       </c>
       <c r="F4" t="n">
-        <v>72.05003413768438</v>
+        <v>66.78241823603955</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1553,19 +1553,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>76.71185306724166</v>
+        <v>71.19693742826449</v>
       </c>
       <c r="C5" t="n">
-        <v>77.15129459938419</v>
+        <v>71.19693742826448</v>
       </c>
       <c r="D5" t="n">
-        <v>71.29769818799942</v>
+        <v>95.78875809923618</v>
       </c>
       <c r="E5" t="n">
-        <v>68.70118377780271</v>
+        <v>85.71201610437265</v>
       </c>
       <c r="F5" t="n">
-        <v>77.134466150836</v>
+        <v>71.34859564869012</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1573,19 +1573,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>76.71185306724166</v>
+        <v>71.19693742826449</v>
       </c>
       <c r="C6" t="n">
-        <v>77.03193930128623</v>
+        <v>71.19693742826449</v>
       </c>
       <c r="D6" t="n">
-        <v>67.54118218901277</v>
+        <v>96.01549215969001</v>
       </c>
       <c r="E6" t="n">
-        <v>61.16654417278157</v>
+        <v>83.96529040486715</v>
       </c>
       <c r="F6" t="n">
-        <v>77.01258581222952</v>
+        <v>71.26091112062491</v>
       </c>
     </row>
   </sheetData>
@@ -1629,19 +1629,19 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>32.2585906481</v>
+        <v>58.59806556420001</v>
       </c>
       <c r="C2" t="n">
-        <v>32.804257895</v>
+        <v>58.5980655644</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6778251844999977</v>
+        <v>16.5200310559</v>
       </c>
       <c r="E2" t="n">
-        <v>1.205243237000001</v>
+        <v>1.516094787630001</v>
       </c>
       <c r="F2" t="n">
-        <v>33.0996980379</v>
+        <v>58.59806556839999</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1649,19 +1649,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>44.7150128706</v>
+        <v>45.1898817245</v>
       </c>
       <c r="C3" t="n">
-        <v>44.8231193247</v>
+        <v>45.18988172469999</v>
       </c>
       <c r="D3" t="n">
-        <v>1.458743322400001</v>
+        <v>12.8415761722</v>
       </c>
       <c r="E3" t="n">
-        <v>2.589915539699999</v>
+        <v>1.457375900210002</v>
       </c>
       <c r="F3" t="n">
-        <v>45.1435567131</v>
+        <v>45.1898825652</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1669,19 +1669,19 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>66.6162793579</v>
+        <v>31.3573040324</v>
       </c>
       <c r="C4" t="n">
-        <v>70.7340138779</v>
+        <v>31.35730403243</v>
       </c>
       <c r="D4" t="n">
-        <v>2.098170737499997</v>
+        <v>9.736506157199997</v>
       </c>
       <c r="E4" t="n">
-        <v>3.751754783700002</v>
+        <v>1.455261540899999</v>
       </c>
       <c r="F4" t="n">
-        <v>73.7791115592</v>
+        <v>31.3861885265351</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1689,19 +1689,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>179.9064077958452</v>
+        <v>212.0886596067572</v>
       </c>
       <c r="C5" t="n">
-        <v>219.5544999999999</v>
+        <v>212.0886596067572</v>
       </c>
       <c r="D5" t="n">
-        <v>11.5802727642213</v>
+        <v>36.64749990315177</v>
       </c>
       <c r="E5" t="n">
-        <v>5.123833180861053</v>
+        <v>7.263342628703831</v>
       </c>
       <c r="F5" t="n">
-        <v>219.6302134448778</v>
+        <v>213.1577006153055</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1709,19 +1709,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>179.9064077958452</v>
+        <v>212.0886596067572</v>
       </c>
       <c r="C6" t="n">
-        <v>229.8651666666666</v>
+        <v>212.0886596067571</v>
       </c>
       <c r="D6" t="n">
-        <v>9.070421508292783</v>
+        <v>36.25249688483122</v>
       </c>
       <c r="E6" t="n">
-        <v>4.248864228360006</v>
+        <v>4.574089969523367</v>
       </c>
       <c r="F6" t="n">
-        <v>229.9223095256634</v>
+        <v>212.0891038629994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up and documented files
</commit_message>
<xml_diff>
--- a/misc/FlexibiltyFunctions/results/tables.xlsx
+++ b/misc/FlexibiltyFunctions/results/tables.xlsx
@@ -2,29 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="10" firstSheet="9" windowHeight="6870" windowWidth="19155" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitances kWhperK" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Downward energy kWh" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Upward Energy kWh" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Max upward power kW" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Stored energy vs capacitance" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Response time" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="efficiency percent" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Downward energy kWh" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Upward Energy kWh" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Max upward power kW" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Stored energy vs capacitance" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Energy difference kWh" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="efficciency percent" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Max downward power kW" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Cost difference euro" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Max downward power kW" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Cost difference euro" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="UAvalues" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Table 3" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Table 4" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Table 5" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId14"/>
+  </externalReferences>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Network</t>
   </si>
@@ -35,31 +40,49 @@
     <t>Combined</t>
   </si>
   <si>
-    <t>NewStreet</t>
+    <t>Terraced street</t>
   </si>
   <si>
-    <t>MixedStreet</t>
+    <t>Mixed street</t>
   </si>
   <si>
-    <t>OldStreet</t>
+    <t>Detached street</t>
   </si>
   <si>
-    <t>linear</t>
+    <t>Series</t>
   </si>
   <si>
-    <t>radial</t>
+    <t>Parallel</t>
   </si>
   <si>
-    <t>NoPipes</t>
+    <t>Buildings - ideal network</t>
   </si>
   <si>
-    <t>Building</t>
+    <t>Combined - LP</t>
   </si>
   <si>
-    <t>Pipe</t>
+    <t>Combined - LP total</t>
   </si>
   <si>
-    <t>Combined total</t>
+    <t>Capacitances [kWh/K]</t>
+  </si>
+  <si>
+    <t>UA values [W/K]</t>
+  </si>
+  <si>
+    <t>Building UA values</t>
+  </si>
+  <si>
+    <t>Stored</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Stored energy</t>
+  </si>
+  <si>
+    <t>Used energy</t>
   </si>
 </sst>
 </file>
@@ -67,9 +90,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="[hh]:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="0.0" numFmtId="164"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,23 +101,233 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.7999816888943144"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -108,18 +341,965 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="11" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="12" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="13" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Buildings</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Table 5'!$B$10</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Stored energy</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'[1]Downward energy kWh'!$B$21:$B$25</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Terraced street</v>
+                </pt>
+                <pt idx="1">
+                  <v>Mixed street</v>
+                </pt>
+                <pt idx="2">
+                  <v>Detached street</v>
+                </pt>
+                <pt idx="3">
+                  <v>Series district</v>
+                </pt>
+                <pt idx="4">
+                  <v>Parallel district</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Table 5'!$D$3:$D$7</f>
+              <numCache>
+                <formatCode>0</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>802.1713472015626</v>
+                </pt>
+                <pt idx="1">
+                  <v>1040.572929647893</v>
+                </pt>
+                <pt idx="2">
+                  <v>1227.385245305097</v>
+                </pt>
+                <pt idx="3">
+                  <v>2989.04718953229</v>
+                </pt>
+                <pt idx="4">
+                  <v>2900.075486929875</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Table 5'!$B$11</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Used energy</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'[1]Downward energy kWh'!$B$21:$B$25</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Terraced street</v>
+                </pt>
+                <pt idx="1">
+                  <v>Mixed street</v>
+                </pt>
+                <pt idx="2">
+                  <v>Detached street</v>
+                </pt>
+                <pt idx="3">
+                  <v>Series district</v>
+                </pt>
+                <pt idx="4">
+                  <v>Parallel district</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Table 5'!$E$3:$E$7</f>
+              <numCache>
+                <formatCode>0</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>594.6833793240844</v>
+                </pt>
+                <pt idx="1">
+                  <v>798.7529861847767</v>
+                </pt>
+                <pt idx="2">
+                  <v>971.8796275298116</v>
+                </pt>
+                <pt idx="3">
+                  <v>2329.242976315842</v>
+                </pt>
+                <pt idx="4">
+                  <v>2281.108570783984</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="494916568"/>
+        <axId val="494914272"/>
+      </barChart>
+      <catAx>
+        <axId val="494916568"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill/>
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="494914272"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="494914272"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="494916568"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+      <txPr>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:t>None</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </txPr>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Network</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Table 5'!$B$10</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Stored energy</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'[1]Downward energy kWh'!$B$21:$B$25</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Terraced street</v>
+                </pt>
+                <pt idx="1">
+                  <v>Mixed street</v>
+                </pt>
+                <pt idx="2">
+                  <v>Detached street</v>
+                </pt>
+                <pt idx="3">
+                  <v>Series district</v>
+                </pt>
+                <pt idx="4">
+                  <v>Parallel district</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Table 5'!$F$3:$F$7</f>
+              <numCache>
+                <formatCode>0.00</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.691697448908333</v>
+                </pt>
+                <pt idx="1">
+                  <v>3.233562733632835</v>
+                </pt>
+                <pt idx="2">
+                  <v>3.919872602102084</v>
+                </pt>
+                <pt idx="3">
+                  <v>12.88055761046826</v>
+                </pt>
+                <pt idx="4">
+                  <v>7.619046943279084</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Table 5'!$B$11</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>Used energy</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>'[1]Downward energy kWh'!$B$21:$B$25</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Terraced street</v>
+                </pt>
+                <pt idx="1">
+                  <v>Mixed street</v>
+                </pt>
+                <pt idx="2">
+                  <v>Detached street</v>
+                </pt>
+                <pt idx="3">
+                  <v>Series district</v>
+                </pt>
+                <pt idx="4">
+                  <v>Parallel district</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Table 5'!$G$3:$G$7</f>
+              <numCache>
+                <formatCode>0.00</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.3514007368333344</v>
+                </pt>
+                <pt idx="1">
+                  <v>1.920314611367418</v>
+                </pt>
+                <pt idx="2">
+                  <v>2.620385724402252</v>
+                </pt>
+                <pt idx="3">
+                  <v>7.949476573613008</v>
+                </pt>
+                <pt idx="4">
+                  <v>4.157717934689749</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="494916568"/>
+        <axId val="494914272"/>
+      </barChart>
+      <catAx>
+        <axId val="494916568"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill/>
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="494914272"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="494914272"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0.00" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="494916568"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+      <txPr>
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:t>None</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </txPr>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>733425</colOff>
+      <row>12</row>
+      <rowOff>133350</rowOff>
+    </from>
+    <to>
+      <col>7</col>
+      <colOff>609040</colOff>
+      <row>27</row>
+      <rowOff>19050</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor>
+    <from>
+      <col>8</col>
+      <colOff>114300</colOff>
+      <row>12</row>
+      <rowOff>123825</rowOff>
+    </from>
+    <to>
+      <col>15</col>
+      <colOff>399490</colOff>
+      <row>27</row>
+      <rowOff>9525</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook r:id="rId1">
+    <sheetNames>
+      <sheetName val="Capacitances kWhperK"/>
+      <sheetName val="Downward energy kWh"/>
+      <sheetName val="Upward Energy kWh"/>
+      <sheetName val="Max upward power kW"/>
+      <sheetName val="Stored energy vs capacitance"/>
+      <sheetName val="Response time"/>
+      <sheetName val="Energy difference kWh"/>
+      <sheetName val="efficciency percent"/>
+      <sheetName val="Max downward power kW"/>
+      <sheetName val="Cost difference euro"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="21">
+          <cell r="B21" t="str">
+            <v>Terraced street</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Mixed street</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v>Detached street</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v>Series district</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>Parallel district</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,90 +1594,90 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4171048047185274</v>
+        <v>0.3870335217262679</v>
       </c>
       <c r="C2" t="n">
         <v>292.2374272270289</v>
       </c>
       <c r="D2" t="n">
-        <v>292.6545320317474</v>
+        <v>292.6244607487552</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4171048047185274</v>
+        <v>0.4020691632223977</v>
       </c>
       <c r="C3" t="n">
-        <v>390.57361416907</v>
+        <v>338.9701910579588</v>
       </c>
       <c r="D3" t="n">
-        <v>390.9907189737885</v>
+        <v>339.3722602211812</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4924923276165055</v>
+        <v>0.4020691632223977</v>
       </c>
       <c r="C4" t="n">
-        <v>488.9098011111111</v>
+        <v>385.7029548888888</v>
       </c>
       <c r="D4" t="n">
-        <v>489.4022934387276</v>
+        <v>386.1050240521112</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7530437207447092</v>
+        <v>0.9650701014963002</v>
       </c>
       <c r="C5" t="n">
-        <v>1020.082578953735</v>
+        <v>944.0555501159179</v>
       </c>
       <c r="D5" t="n">
-        <v>1020.83562267448</v>
+        <v>945.0206202174141</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5955640062407849</v>
+        <v>0.5373899366875651</v>
       </c>
       <c r="C6" t="n">
-        <v>1020.082578953735</v>
+        <v>944.0555501159179</v>
       </c>
       <c r="D6" t="n">
-        <v>1020.678142959976</v>
+        <v>944.5929400526054</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +1691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,125 +1699,708 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>385.7964956788765</v>
-      </c>
-      <c r="C2" t="n">
-        <v>387.2329386709962</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.01110402476751915</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.09746728546178929</v>
-      </c>
-      <c r="F2" t="n">
-        <v>387.330405956458</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+        <v>36.40057259440879</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>380.7882839622944</v>
-      </c>
-      <c r="C3" t="n">
-        <v>380.5221840208742</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.2300238905081642</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6477143322636039</v>
-      </c>
-      <c r="F3" t="n">
-        <v>381.1698983531378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+        <v>36.59612862665554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>372.0174581982956</v>
-      </c>
-      <c r="C4" t="n">
-        <v>372.7242787690247</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.3873981816668675</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.091930966353175</v>
-      </c>
-      <c r="F4" t="n">
-        <v>373.8162097353779</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+        <v>36.59612862665554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>1669.758733198825</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1760.191479449491</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.32724134140517</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.419278736753768</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1762.610758186245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+        <v>43.69529417146323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>1669.758733198825</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1741.192818311793</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.039757154663675</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8784699928692135</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1742.071288304662</v>
+        <v>38.35613291687628</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="45" width="13.85546875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="45" width="8"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="45" width="7.85546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="45" width="9"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="45" width="8"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="45" width="7.85546875"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="45" width="9"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="43" width="15.28515625"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="43" spans="1:12" thickBot="1">
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="43" spans="1:12" thickBot="1">
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="23">
+        <f>'Capacitances kWhperK'!B1</f>
+        <v/>
+      </c>
+      <c r="C2" s="24">
+        <f>'Capacitances kWhperK'!C1</f>
+        <v/>
+      </c>
+      <c r="D2" s="24">
+        <f>'Capacitances kWhperK'!D1</f>
+        <v/>
+      </c>
+      <c r="E2" s="24">
+        <f>'Capacitances kWhperK'!B1</f>
+        <v/>
+      </c>
+      <c r="F2" s="24">
+        <f>'Capacitances kWhperK'!C1</f>
+        <v/>
+      </c>
+      <c r="G2" s="25">
+        <f>'Capacitances kWhperK'!D1</f>
+        <v/>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="44">
+        <f>'Capacitances kWhperK'!A2</f>
+        <v/>
+      </c>
+      <c r="B3" s="18">
+        <f>'Capacitances kWhperK'!B2</f>
+        <v/>
+      </c>
+      <c r="C3" s="19">
+        <f>'Capacitances kWhperK'!C2</f>
+        <v/>
+      </c>
+      <c r="D3" s="19">
+        <f>'Capacitances kWhperK'!D2</f>
+        <v/>
+      </c>
+      <c r="E3" s="20">
+        <f>UAvalues!B2</f>
+        <v/>
+      </c>
+      <c r="F3" s="21">
+        <f>10*L3</f>
+        <v/>
+      </c>
+      <c r="G3" s="22">
+        <f>SUM(E3:F3)</f>
+        <v/>
+      </c>
+      <c r="K3" s="2">
+        <f>A3</f>
+        <v/>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5">
+        <f>'Capacitances kWhperK'!A3</f>
+        <v/>
+      </c>
+      <c r="B4" s="15">
+        <f>'Capacitances kWhperK'!B3</f>
+        <v/>
+      </c>
+      <c r="C4" s="6">
+        <f>'Capacitances kWhperK'!C3</f>
+        <v/>
+      </c>
+      <c r="D4" s="6">
+        <f>'Capacitances kWhperK'!D3</f>
+        <v/>
+      </c>
+      <c r="E4" s="7">
+        <f>UAvalues!B3</f>
+        <v/>
+      </c>
+      <c r="F4" s="8">
+        <f>5*L3 + 5*L5</f>
+        <v/>
+      </c>
+      <c r="G4" s="9">
+        <f>SUM(E4:F4)</f>
+        <v/>
+      </c>
+      <c r="K4" s="2">
+        <f>A4</f>
+        <v/>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="5">
+        <f>'Capacitances kWhperK'!A4</f>
+        <v/>
+      </c>
+      <c r="B5" s="15">
+        <f>'Capacitances kWhperK'!B4</f>
+        <v/>
+      </c>
+      <c r="C5" s="6">
+        <f>'Capacitances kWhperK'!C4</f>
+        <v/>
+      </c>
+      <c r="D5" s="6">
+        <f>'Capacitances kWhperK'!D4</f>
+        <v/>
+      </c>
+      <c r="E5" s="7">
+        <f>UAvalues!B4</f>
+        <v/>
+      </c>
+      <c r="F5" s="8">
+        <f>10*L5</f>
+        <v/>
+      </c>
+      <c r="G5" s="9">
+        <f>SUM(E5:F5)</f>
+        <v/>
+      </c>
+      <c r="K5" s="2">
+        <f>A5</f>
+        <v/>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="5">
+        <f>'Capacitances kWhperK'!A5</f>
+        <v/>
+      </c>
+      <c r="B6" s="15">
+        <f>'Capacitances kWhperK'!B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="6">
+        <f>'Capacitances kWhperK'!C5</f>
+        <v/>
+      </c>
+      <c r="D6" s="6">
+        <f>'Capacitances kWhperK'!D5</f>
+        <v/>
+      </c>
+      <c r="E6" s="7">
+        <f>UAvalues!B5</f>
+        <v/>
+      </c>
+      <c r="F6" s="8">
+        <f>10*SUM(L3:L5)</f>
+        <v/>
+      </c>
+      <c r="G6" s="9">
+        <f>SUM(E6:F6)</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="43" spans="1:12" thickBot="1">
+      <c r="A7" s="10">
+        <f>'Capacitances kWhperK'!A6</f>
+        <v/>
+      </c>
+      <c r="B7" s="16">
+        <f>'Capacitances kWhperK'!B6</f>
+        <v/>
+      </c>
+      <c r="C7" s="11">
+        <f>'Capacitances kWhperK'!C6</f>
+        <v/>
+      </c>
+      <c r="D7" s="11">
+        <f>'Capacitances kWhperK'!D6</f>
+        <v/>
+      </c>
+      <c r="E7" s="12">
+        <f>UAvalues!B6</f>
+        <v/>
+      </c>
+      <c r="F7" s="13">
+        <f>10*SUM(L3:L5)</f>
+        <v/>
+      </c>
+      <c r="G7" s="14">
+        <f>SUM(E7:F7)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="43" width="13.28515625"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15.75" r="1" s="43" spans="1:4" thickBot="1">
+      <c r="A1" s="28" t="n"/>
+      <c r="B1" s="24">
+        <f>'Table 3'!B2</f>
+        <v/>
+      </c>
+      <c r="C1" s="24">
+        <f>'Table 3'!C2</f>
+        <v/>
+      </c>
+      <c r="D1" s="25">
+        <f>'Table 3'!D2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="29">
+        <f>'Table 3'!A3</f>
+        <v/>
+      </c>
+      <c r="B2" s="7">
+        <f>'Table 3'!B3/'Table 3'!E3*1000</f>
+        <v/>
+      </c>
+      <c r="C2" s="7">
+        <f>'Table 3'!C3/'Table 3'!F3*100</f>
+        <v/>
+      </c>
+      <c r="D2" s="30">
+        <f>'Table 3'!D3/'Table 3'!G3*100</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="29">
+        <f>'Table 3'!A4</f>
+        <v/>
+      </c>
+      <c r="B3" s="7">
+        <f>'Table 3'!B4/'Table 3'!E4*1000</f>
+        <v/>
+      </c>
+      <c r="C3" s="7">
+        <f>'Table 3'!C4/'Table 3'!F4*100</f>
+        <v/>
+      </c>
+      <c r="D3" s="30">
+        <f>'Table 3'!D4/'Table 3'!G4*100</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="29">
+        <f>'Table 3'!A5</f>
+        <v/>
+      </c>
+      <c r="B4" s="7">
+        <f>'Table 3'!B5/'Table 3'!E5*1000</f>
+        <v/>
+      </c>
+      <c r="C4" s="7">
+        <f>'Table 3'!C5/'Table 3'!F5*100</f>
+        <v/>
+      </c>
+      <c r="D4" s="30">
+        <f>'Table 3'!D5/'Table 3'!G5*100</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="29">
+        <f>'Table 3'!A6</f>
+        <v/>
+      </c>
+      <c r="B5" s="7">
+        <f>'Table 3'!B6/'Table 3'!E6*1000</f>
+        <v/>
+      </c>
+      <c r="C5" s="7">
+        <f>'Table 3'!C6/'Table 3'!F6*100</f>
+        <v/>
+      </c>
+      <c r="D5" s="30">
+        <f>'Table 3'!D6/'Table 3'!G6*100</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="43" spans="1:4" thickBot="1">
+      <c r="A6" s="31">
+        <f>'Table 3'!A7</f>
+        <v/>
+      </c>
+      <c r="B6" s="12">
+        <f>'Table 3'!B7/'Table 3'!E7*1000</f>
+        <v/>
+      </c>
+      <c r="C6" s="12">
+        <f>'Table 3'!C7/'Table 3'!F7*100</f>
+        <v/>
+      </c>
+      <c r="D6" s="32">
+        <f>'Table 3'!D7/'Table 3'!G7*100</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="43" width="13.85546875"/>
+    <col customWidth="1" max="2" min="2" style="43" width="6.85546875"/>
+    <col customWidth="1" max="3" min="3" style="43" width="6.42578125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="43" width="6.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="43" width="5"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="43" width="6.28515625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="43" width="4.85546875"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="43" width="6.28515625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="43" width="5"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="29.25" r="1" s="43" spans="1:9" thickBot="1">
+      <c r="A1" s="39" t="n"/>
+      <c r="B1" s="47">
+        <f>'Cost difference euro'!B1</f>
+        <v/>
+      </c>
+      <c r="D1" s="48">
+        <f>'Cost difference euro'!C1</f>
+        <v/>
+      </c>
+      <c r="F1" s="48">
+        <f>'Cost difference euro'!D1</f>
+        <v/>
+      </c>
+      <c r="H1" s="48">
+        <f>'Cost difference euro'!E1</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="43" spans="1:9" thickBot="1">
+      <c r="A2" s="40" t="n"/>
+      <c r="B2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="26">
+        <f>'Table 4'!A2</f>
+        <v/>
+      </c>
+      <c r="B3" s="33">
+        <f>'Upward Energy kWh'!B2</f>
+        <v/>
+      </c>
+      <c r="C3" s="33">
+        <f>'Downward energy kWh'!B2</f>
+        <v/>
+      </c>
+      <c r="D3" s="33">
+        <f>'Upward Energy kWh'!C2</f>
+        <v/>
+      </c>
+      <c r="E3" s="33">
+        <f>'Downward energy kWh'!C2</f>
+        <v/>
+      </c>
+      <c r="F3" s="34">
+        <f>'Upward Energy kWh'!D2</f>
+        <v/>
+      </c>
+      <c r="G3" s="34">
+        <f>'Downward energy kWh'!D2</f>
+        <v/>
+      </c>
+      <c r="H3" s="33">
+        <f>'Upward Energy kWh'!F2</f>
+        <v/>
+      </c>
+      <c r="I3" s="35">
+        <f>'Downward energy kWh'!F2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="26">
+        <f>'Table 4'!A3</f>
+        <v/>
+      </c>
+      <c r="B4" s="33">
+        <f>'Upward Energy kWh'!B3</f>
+        <v/>
+      </c>
+      <c r="C4" s="33">
+        <f>'Downward energy kWh'!B3</f>
+        <v/>
+      </c>
+      <c r="D4" s="33">
+        <f>'Upward Energy kWh'!C3</f>
+        <v/>
+      </c>
+      <c r="E4" s="33">
+        <f>'Downward energy kWh'!C3</f>
+        <v/>
+      </c>
+      <c r="F4" s="34">
+        <f>'Upward Energy kWh'!D3</f>
+        <v/>
+      </c>
+      <c r="G4" s="34">
+        <f>'Downward energy kWh'!D3</f>
+        <v/>
+      </c>
+      <c r="H4" s="33">
+        <f>'Upward Energy kWh'!F3</f>
+        <v/>
+      </c>
+      <c r="I4" s="35">
+        <f>'Downward energy kWh'!F3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="26">
+        <f>'Table 4'!A4</f>
+        <v/>
+      </c>
+      <c r="B5" s="33">
+        <f>'Upward Energy kWh'!B4</f>
+        <v/>
+      </c>
+      <c r="C5" s="33">
+        <f>'Downward energy kWh'!B4</f>
+        <v/>
+      </c>
+      <c r="D5" s="33">
+        <f>'Upward Energy kWh'!C4</f>
+        <v/>
+      </c>
+      <c r="E5" s="33">
+        <f>'Downward energy kWh'!C4</f>
+        <v/>
+      </c>
+      <c r="F5" s="34">
+        <f>'Upward Energy kWh'!D4</f>
+        <v/>
+      </c>
+      <c r="G5" s="34">
+        <f>'Downward energy kWh'!D4</f>
+        <v/>
+      </c>
+      <c r="H5" s="33">
+        <f>'Upward Energy kWh'!F4</f>
+        <v/>
+      </c>
+      <c r="I5" s="35">
+        <f>'Downward energy kWh'!F4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="26">
+        <f>'Table 4'!A5</f>
+        <v/>
+      </c>
+      <c r="B6" s="33">
+        <f>'Upward Energy kWh'!B5</f>
+        <v/>
+      </c>
+      <c r="C6" s="33">
+        <f>'Downward energy kWh'!B5</f>
+        <v/>
+      </c>
+      <c r="D6" s="33">
+        <f>'Upward Energy kWh'!C5</f>
+        <v/>
+      </c>
+      <c r="E6" s="33">
+        <f>'Downward energy kWh'!C5</f>
+        <v/>
+      </c>
+      <c r="F6" s="34">
+        <f>'Upward Energy kWh'!D5</f>
+        <v/>
+      </c>
+      <c r="G6" s="34">
+        <f>'Downward energy kWh'!D5</f>
+        <v/>
+      </c>
+      <c r="H6" s="33">
+        <f>'Upward Energy kWh'!F5</f>
+        <v/>
+      </c>
+      <c r="I6" s="35">
+        <f>'Downward energy kWh'!F5</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="43" spans="1:9" thickBot="1">
+      <c r="A7" s="27">
+        <f>'Table 4'!A6</f>
+        <v/>
+      </c>
+      <c r="B7" s="36">
+        <f>'Upward Energy kWh'!B6</f>
+        <v/>
+      </c>
+      <c r="C7" s="36">
+        <f>'Downward energy kWh'!B6</f>
+        <v/>
+      </c>
+      <c r="D7" s="36">
+        <f>'Upward Energy kWh'!C6</f>
+        <v/>
+      </c>
+      <c r="E7" s="36">
+        <f>'Downward energy kWh'!C6</f>
+        <v/>
+      </c>
+      <c r="F7" s="37">
+        <f>'Upward Energy kWh'!D6</f>
+        <v/>
+      </c>
+      <c r="G7" s="37">
+        <f>'Downward energy kWh'!D6</f>
+        <v/>
+      </c>
+      <c r="H7" s="36">
+        <f>'Upward Energy kWh'!F6</f>
+        <v/>
+      </c>
+      <c r="I7" s="38">
+        <f>'Downward energy kWh'!F6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -656,120 +2419,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>579.5140426636555</v>
+        <v>74.93117212395831</v>
       </c>
       <c r="C2" t="n">
-        <v>594.6934396468271</v>
+        <v>74.13420853262117</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3514007368333344</v>
+        <v>50.80266478933871</v>
       </c>
       <c r="E2" t="n">
-        <v>2.267358456956484</v>
+        <v>51.09508454186413</v>
       </c>
       <c r="F2" t="n">
-        <v>596.9607981037835</v>
+        <v>74.00746747018469</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>597.4305958031335</v>
+        <v>77.74828377257418</v>
       </c>
       <c r="C3" t="n">
-        <v>602.604524868644</v>
+        <v>76.76088464595074</v>
       </c>
       <c r="D3" t="n">
-        <v>1.541971013309421</v>
+        <v>59.3869601105935</v>
       </c>
       <c r="E3" t="n">
-        <v>3.053954837389351</v>
+        <v>54.24322428635598</v>
       </c>
       <c r="F3" t="n">
-        <v>605.6584797060334</v>
+        <v>76.64244102249292</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>606.4448700444664</v>
+        <v>79.49200272397303</v>
       </c>
       <c r="C4" t="n">
-        <v>607.2282963562053</v>
+        <v>79.18293227383835</v>
       </c>
       <c r="D4" t="n">
-        <v>1.878959421050163</v>
+        <v>66.84874713347949</v>
       </c>
       <c r="E4" t="n">
-        <v>3.507054537282813</v>
+        <v>56.97418144584015</v>
       </c>
       <c r="F4" t="n">
-        <v>610.7353508934881</v>
+        <v>79.07439178449103</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>2397.630113425227</v>
+        <v>78.23405064050971</v>
       </c>
       <c r="C5" t="n">
-        <v>2500.820925594765</v>
+        <v>77.6735367598296</v>
       </c>
       <c r="D5" t="n">
-        <v>3.895419806220104</v>
+        <v>69.01931592242941</v>
       </c>
       <c r="E5" t="n">
-        <v>4.443764496491101</v>
+        <v>65.99591721697486</v>
       </c>
       <c r="F5" t="n">
-        <v>2505.264690091255</v>
+        <v>77.62496190833428</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>2397.630113425227</v>
+        <v>78.23405064050971</v>
       </c>
       <c r="C6" t="n">
-        <v>2480.907085448521</v>
+        <v>78.43443691549861</v>
       </c>
       <c r="D6" t="n">
-        <v>2.001758678579358</v>
+        <v>67.25220090494226</v>
       </c>
       <c r="E6" t="n">
-        <v>2.405980433065935</v>
+        <v>58.39487671924343</v>
       </c>
       <c r="F6" t="n">
-        <v>2483.313065881587</v>
+        <v>78.3827195515894</v>
       </c>
     </row>
   </sheetData>
@@ -792,120 +2555,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>773.2315896484323</v>
+        <v>579.386693198205</v>
       </c>
       <c r="C2" t="n">
-        <v>802.1539406226625</v>
+        <v>594.6833793240844</v>
       </c>
       <c r="D2" t="n">
-        <v>0.691697448908333</v>
+        <v>0.3514007368333344</v>
       </c>
       <c r="E2" t="n">
-        <v>4.437249628458333</v>
+        <v>2.267218372136677</v>
       </c>
       <c r="F2" t="n">
-        <v>806.5911902511208</v>
+        <v>596.9505976962211</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>814.0729076439725</v>
+        <v>770.4282411295119</v>
       </c>
       <c r="C3" t="n">
-        <v>824.6868657164251</v>
+        <v>798.7529861847767</v>
       </c>
       <c r="D3" t="n">
-        <v>2.853918136107166</v>
+        <v>1.920314611367418</v>
       </c>
       <c r="E3" t="n">
-        <v>5.460195342508333</v>
+        <v>2.984673801109532</v>
       </c>
       <c r="F3" t="n">
-        <v>830.1470610589334</v>
+        <v>801.7376599858862</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>840.8722818906374</v>
+        <v>946.4233242348568</v>
       </c>
       <c r="C4" t="n">
-        <v>841.7323139433398</v>
+        <v>971.8796275298116</v>
       </c>
       <c r="D4" t="n">
-        <v>3.370520660430584</v>
+        <v>2.620385724402252</v>
       </c>
       <c r="E4" t="n">
-        <v>5.922178108224999</v>
+        <v>3.43442756330456</v>
       </c>
       <c r="F4" t="n">
-        <v>847.6544920515648</v>
+        <v>975.3140550931162</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>3125.501493651601</v>
+        <v>2299.183368395687</v>
       </c>
       <c r="C5" t="n">
-        <v>3241.450371740041</v>
+        <v>2385.225653178899</v>
       </c>
       <c r="D5" t="n">
-        <v>5.463598271062825</v>
+        <v>7.716248571318497</v>
       </c>
       <c r="E5" t="n">
-        <v>6.468250256322169</v>
+        <v>8.465271710297673</v>
       </c>
       <c r="F5" t="n">
-        <v>3247.918621996364</v>
+        <v>2393.690924889197</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>3125.501493651601</v>
+        <v>2299.183368395687</v>
       </c>
       <c r="C6" t="n">
-        <v>3220.621352585273</v>
+        <v>2371.686208344215</v>
       </c>
       <c r="D6" t="n">
-        <v>2.963760202334127</v>
+        <v>4.405671071409165</v>
       </c>
       <c r="E6" t="n">
-        <v>3.933490873144513</v>
+        <v>4.568731603999917</v>
       </c>
       <c r="F6" t="n">
-        <v>3224.554843458417</v>
+        <v>2376.254939948215</v>
       </c>
     </row>
   </sheetData>
@@ -928,120 +2691,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>70</v>
+        <v>773.2251835577573</v>
       </c>
       <c r="C2" t="n">
-        <v>53.88716666669</v>
+        <v>802.1713472015626</v>
       </c>
       <c r="D2" t="n">
-        <v>2.943590311099999</v>
+        <v>0.691697448908333</v>
       </c>
       <c r="E2" t="n">
-        <v>12.2449672142</v>
+        <v>4.437253391308333</v>
       </c>
       <c r="F2" t="n">
-        <v>53.88716666669</v>
+        <v>806.608600592871</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>48.2907908253</v>
+        <v>990.9263635739622</v>
       </c>
       <c r="C3" t="n">
-        <v>60.88716666663</v>
+        <v>1040.572929647893</v>
       </c>
       <c r="D3" t="n">
-        <v>3.8747372617</v>
+        <v>3.233562733632835</v>
       </c>
       <c r="E3" t="n">
-        <v>15.3400650467</v>
+        <v>5.502390095416668</v>
       </c>
       <c r="F3" t="n">
-        <v>61.48092148843</v>
+        <v>1046.075319743309</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>60.16015098690001</v>
+        <v>1190.58935717145</v>
       </c>
       <c r="C4" t="n">
-        <v>65.8785199453</v>
+        <v>1227.385245305097</v>
       </c>
       <c r="D4" t="n">
-        <v>3.7164204379</v>
+        <v>3.919872602102084</v>
       </c>
       <c r="E4" t="n">
-        <v>18.38280532280001</v>
+        <v>6.028041957916669</v>
       </c>
       <c r="F4" t="n">
-        <v>73.75210118788</v>
+        <v>1233.413287263014</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>190.1922358870569</v>
+        <v>2938.852519550336</v>
       </c>
       <c r="C5" t="n">
-        <v>219.5545</v>
+        <v>3070.834357077569</v>
       </c>
       <c r="D5" t="n">
-        <v>8.612486212553341</v>
+        <v>11.17983924862508</v>
       </c>
       <c r="E5" t="n">
-        <v>39.25682347170054</v>
+        <v>12.82696273741666</v>
       </c>
       <c r="F5" t="n">
-        <v>219.5545</v>
+        <v>3083.661319814985</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>190.1922358870569</v>
+        <v>2938.852519550336</v>
       </c>
       <c r="C6" t="n">
-        <v>225.6276508430201</v>
+        <v>3023.781774450129</v>
       </c>
       <c r="D6" t="n">
-        <v>8.689659568871313</v>
+        <v>6.55096935335075</v>
       </c>
       <c r="E6" t="n">
-        <v>32.94317456523864</v>
+        <v>7.823856920499997</v>
       </c>
       <c r="F6" t="n">
-        <v>225.6276508430201</v>
+        <v>3031.605631370629</v>
       </c>
     </row>
   </sheetData>
@@ -1064,120 +2827,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>2.645901987933038</v>
+        <v>70</v>
       </c>
       <c r="C2" t="n">
-        <v>2.744870662988343</v>
+        <v>53.88716666669</v>
       </c>
       <c r="D2" t="n">
-        <v>1.658330091342648</v>
+        <v>2.943590311099999</v>
       </c>
       <c r="E2" t="n">
-        <v>10.63821269441549</v>
+        <v>12.2450449693</v>
       </c>
       <c r="F2" t="n">
-        <v>2.756120619938396</v>
+        <v>53.88716666669</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>2.084300828605334</v>
+        <v>90</v>
       </c>
       <c r="C3" t="n">
-        <v>2.111476136120752</v>
+        <v>71.88716666662999</v>
       </c>
       <c r="D3" t="n">
-        <v>6.842208729849229</v>
+        <v>4.639430903100001</v>
       </c>
       <c r="E3" t="n">
-        <v>13.09070353719135</v>
+        <v>16.4076218801</v>
       </c>
       <c r="F3" t="n">
-        <v>2.123188660942577</v>
+        <v>71.88716666662999</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>1.719892462739846</v>
+        <v>110</v>
       </c>
       <c r="C4" t="n">
-        <v>1.721651543966584</v>
+        <v>87.98900001137999</v>
       </c>
       <c r="D4" t="n">
-        <v>6.843803388253278</v>
+        <v>5.332534871099997</v>
       </c>
       <c r="E4" t="n">
-        <v>12.02491445275161</v>
+        <v>20.5679010419</v>
       </c>
       <c r="F4" t="n">
-        <v>1.732019860584674</v>
+        <v>87.98900001137999</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>3.063969092440853</v>
+        <v>229.1108356748</v>
       </c>
       <c r="C5" t="n">
-        <v>3.177635260730253</v>
+        <v>219.5545</v>
       </c>
       <c r="D5" t="n">
-        <v>7.255353335473931</v>
+        <v>11.8080512506</v>
       </c>
       <c r="E5" t="n">
-        <v>8.589475057205853</v>
+        <v>47.989969954</v>
       </c>
       <c r="F5" t="n">
-        <v>3.181627433305241</v>
+        <v>219.5545</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>3.063969092440853</v>
+        <v>229.1108356748</v>
       </c>
       <c r="C6" t="n">
-        <v>3.157216306829352</v>
+        <v>158.78270216482</v>
       </c>
       <c r="D6" t="n">
-        <v>4.976392413372085</v>
+        <v>8.395541340100005</v>
       </c>
       <c r="E6" t="n">
-        <v>6.604648420533012</v>
+        <v>46.50152067999998</v>
       </c>
       <c r="F6" t="n">
-        <v>3.159227877758975</v>
+        <v>198.14268870282</v>
       </c>
     </row>
   </sheetData>
@@ -1200,120 +2963,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>1.177083333333333</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0.06944444444444445</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0.01736111111111111</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>1.177083333333333</v>
+      <c r="B2" t="n">
+        <v>2.645880067090332</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.744930226128716</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.787177105030041</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11.46477796423694</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.756463347352968</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>0.9895833333333334</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>1.0625</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0.02083333333333333</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>1.0625</v>
+      <c r="B3" t="n">
+        <v>2.923343673616801</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.069806599807976</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8.042304731149564</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.68518304492084</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.082383100674003</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0.8541666666666666</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.1145833333333333</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.02083333333333333</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0.8541666666666666</v>
+      <c r="B4" t="n">
+        <v>3.086803826832045</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.182203376322786</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9.749249533801908</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14.99254981308368</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.194502040710417</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>1.291666666666667</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.2048611111111111</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.01736111111111111</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>1.291666666666667</v>
+      <c r="B5" t="n">
+        <v>3.113008041941475</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.252811083733907</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.58448410254469</v>
+      </c>
+      <c r="E5" t="n">
+        <v>13.29122383703422</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.263062470642756</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>1.083333333333333</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>1.291666666666667</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0.2048611111111111</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.01041666666666667</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>1.291666666666667</v>
+      <c r="B6" t="n">
+        <v>3.113008041941475</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.202970179115887</v>
+      </c>
+      <c r="D6" t="n">
+        <v>12.19034616414754</v>
+      </c>
+      <c r="E6" t="n">
+        <v>14.55899410533386</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.209430753528388</v>
       </c>
     </row>
   </sheetData>
@@ -1336,120 +3099,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>193.7175469847807</v>
+        <v>193.8384903595525</v>
       </c>
       <c r="C2" t="n">
-        <v>207.4605009758361</v>
+        <v>207.4879678774778</v>
       </c>
       <c r="D2" t="n">
         <v>0.3402967120746325</v>
       </c>
       <c r="E2" t="n">
-        <v>2.169891171502968</v>
+        <v>2.170035019170427</v>
       </c>
       <c r="F2" t="n">
-        <v>209.6303921473391</v>
+        <v>209.6580028966482</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>216.6423118408402</v>
+        <v>220.4981224444427</v>
       </c>
       <c r="C3" t="n">
-        <v>222.0823408477745</v>
+        <v>241.819943463106</v>
       </c>
       <c r="D3" t="n">
-        <v>1.311947122794663</v>
+        <v>1.313248122267396</v>
       </c>
       <c r="E3" t="n">
-        <v>2.406240505117239</v>
+        <v>2.517716294308229</v>
       </c>
       <c r="F3" t="n">
-        <v>224.4885813528917</v>
+        <v>244.3376597574143</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>234.4274118461808</v>
+        <v>244.166032936585</v>
       </c>
       <c r="C4" t="n">
-        <v>234.5040175871354</v>
+        <v>255.5056177753086</v>
       </c>
       <c r="D4" t="n">
-        <v>1.491561239381554</v>
+        <v>1.299486877697746</v>
       </c>
       <c r="E4" t="n">
-        <v>2.415123570942342</v>
+        <v>2.593614394612814</v>
       </c>
       <c r="F4" t="n">
-        <v>236.9191411580778</v>
+        <v>258.0992321699214</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>727.8713802263755</v>
+        <v>639.6691511546596</v>
       </c>
       <c r="C5" t="n">
-        <v>740.6294461452617</v>
+        <v>685.6087038986479</v>
       </c>
       <c r="D5" t="n">
-        <v>1.568178464840457</v>
+        <v>3.46359067730009</v>
       </c>
       <c r="E5" t="n">
-        <v>2.024485759837262</v>
+        <v>4.361691027119377</v>
       </c>
       <c r="F5" t="n">
-        <v>742.6539319050989</v>
+        <v>689.9703949257673</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>727.8713802263755</v>
+        <v>639.6691511546596</v>
       </c>
       <c r="C6" t="n">
-        <v>739.7142671367492</v>
+        <v>652.0955661058906</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9620015237578627</v>
+        <v>2.145298281946452</v>
       </c>
       <c r="E6" t="n">
-        <v>1.527510440086189</v>
+        <v>3.255125316511112</v>
       </c>
       <c r="F6" t="n">
-        <v>741.2417775768354</v>
+        <v>655.3506914224017</v>
       </c>
     </row>
   </sheetData>
@@ -1472,120 +3235,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>74.94702110222832</v>
+        <v>32.2553681833</v>
       </c>
       <c r="C2" t="n">
-        <v>74.1370713936108</v>
+        <v>32.8090480346</v>
       </c>
       <c r="D2" t="n">
-        <v>50.80266478933871</v>
+        <v>0.6778251844999977</v>
       </c>
       <c r="E2" t="n">
-        <v>51.09828489034696</v>
+        <v>1.2039334858</v>
       </c>
       <c r="F2" t="n">
-        <v>74.01032955953661</v>
+        <v>33.1049723935</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>73.38784894972584</v>
+        <v>56.9625885831</v>
       </c>
       <c r="C3" t="n">
-        <v>73.07070718828733</v>
+        <v>64.88716666662999</v>
       </c>
       <c r="D3" t="n">
-        <v>54.02996649625059</v>
+        <v>1.766921477700002</v>
       </c>
       <c r="E3" t="n">
-        <v>55.93123771698426</v>
+        <v>2.171914873999998</v>
       </c>
       <c r="F3" t="n">
-        <v>72.95797432959979</v>
+        <v>64.90257848801799</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>72.12092527062492</v>
+        <v>85.05611298619999</v>
       </c>
       <c r="C4" t="n">
-        <v>72.14030948993111</v>
+        <v>87.98900000057999</v>
       </c>
       <c r="D4" t="n">
-        <v>55.74685960395976</v>
+        <v>8.157913669000001</v>
       </c>
       <c r="E4" t="n">
-        <v>59.21899802067521</v>
+        <v>2.908554808000001</v>
       </c>
       <c r="F4" t="n">
-        <v>72.05003413768438</v>
+        <v>88.01116461535298</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>76.71185306724166</v>
+        <v>188.8698334343</v>
       </c>
       <c r="C5" t="n">
-        <v>77.15129459938419</v>
+        <v>219.5545</v>
       </c>
       <c r="D5" t="n">
-        <v>71.29769818799942</v>
+        <v>18.250896148</v>
       </c>
       <c r="E5" t="n">
-        <v>68.70118377780271</v>
+        <v>6.793435840399997</v>
       </c>
       <c r="F5" t="n">
-        <v>77.134466150836</v>
+        <v>219.62730456434</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>76.71185306724166</v>
+        <v>188.8698334343</v>
       </c>
       <c r="C6" t="n">
-        <v>77.03193930128623</v>
+        <v>199.75806180816</v>
       </c>
       <c r="D6" t="n">
-        <v>67.54118218901277</v>
+        <v>14.8215640981</v>
       </c>
       <c r="E6" t="n">
-        <v>61.16654417278157</v>
+        <v>5.664693647200002</v>
       </c>
       <c r="F6" t="n">
-        <v>77.01258581222952</v>
+        <v>200.5577828314</v>
       </c>
     </row>
   </sheetData>
@@ -1608,120 +3371,120 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>32.2585906481</v>
+        <v>385.5482028386505</v>
       </c>
       <c r="C2" t="n">
-        <v>32.804257895</v>
+        <v>387.1954114466207</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6778251844999977</v>
+        <v>0.01110402476933814</v>
       </c>
       <c r="E2" t="n">
-        <v>1.205243237000001</v>
+        <v>0.09718335296111036</v>
       </c>
       <c r="F2" t="n">
-        <v>33.0996980379</v>
+        <v>387.2925947995818</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>44.7150128706</v>
+        <v>549.9301186850626</v>
       </c>
       <c r="C3" t="n">
-        <v>44.8231193247</v>
+        <v>556.933042721661</v>
       </c>
       <c r="D3" t="n">
-        <v>1.458743322400001</v>
+        <v>0.6070664890849002</v>
       </c>
       <c r="E3" t="n">
-        <v>2.589915539699999</v>
+        <v>0.4669575067928236</v>
       </c>
       <c r="F3" t="n">
-        <v>45.1435567131</v>
+        <v>557.4000002284538</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>66.6162793579</v>
+        <v>702.2572912982632</v>
       </c>
       <c r="C4" t="n">
-        <v>70.7340138779</v>
+        <v>716.3740097545196</v>
       </c>
       <c r="D4" t="n">
-        <v>2.098170737499997</v>
+        <v>1.320898846741329</v>
       </c>
       <c r="E4" t="n">
-        <v>3.751754783700002</v>
+        <v>0.840813168695604</v>
       </c>
       <c r="F4" t="n">
-        <v>73.7791115592</v>
+        <v>717.2148229232153</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>179.9064077958452</v>
+        <v>1659.514217241023</v>
       </c>
       <c r="C5" t="n">
-        <v>219.5544999999999</v>
+        <v>1699.616949280298</v>
       </c>
       <c r="D5" t="n">
-        <v>11.5802727642213</v>
+        <v>4.252657893928699</v>
       </c>
       <c r="E5" t="n">
-        <v>5.123833180861053</v>
+        <v>4.103580683196924</v>
       </c>
       <c r="F5" t="n">
-        <v>219.6302134448778</v>
+        <v>1703.720529963495</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>179.9064077958452</v>
+        <v>1659.514217241023</v>
       </c>
       <c r="C6" t="n">
-        <v>229.8651666666666</v>
+        <v>1719.590642238294</v>
       </c>
       <c r="D6" t="n">
-        <v>9.070421508292783</v>
+        <v>2.260372789463872</v>
       </c>
       <c r="E6" t="n">
-        <v>4.248864228360006</v>
+        <v>1.313606287490984</v>
       </c>
       <c r="F6" t="n">
-        <v>229.9223095256634</v>
+        <v>1720.904248525785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>